<commit_message>
Minor update to the tests.
</commit_message>
<xml_diff>
--- a/core/tests/resources/glacier snowpack.xlsx
+++ b/core/tests/resources/glacier snowpack.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\Hydrobricks\core\tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\hydrobricks\core\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E59E2C-3534-4F28-B46B-D0DC5ABC8C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CCF1BD-9841-428F-BF4C-B12EAE9E11A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30345" yWindow="4005" windowWidth="18900" windowHeight="10830" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
+    <workbookView xWindow="35325" yWindow="330" windowWidth="18075" windowHeight="16995" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>snow</t>
   </si>
@@ -68,6 +67,12 @@
   </si>
   <si>
     <t>glacier</t>
+  </si>
+  <si>
+    <t>ice degree day</t>
+  </si>
+  <si>
+    <t>ice melting t°</t>
   </si>
 </sst>
 </file>
@@ -429,7 +434,7 @@
   <dimension ref="B1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +469,7 @@
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -472,7 +477,7 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>

<commit_message>
Adding checks that every container has a process.
</commit_message>
<xml_diff>
--- a/core/tests/resources/glacier snowpack.xlsx
+++ b/core/tests/resources/glacier snowpack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\hydrobricks\core\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CCF1BD-9841-428F-BF4C-B12EAE9E11A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8457A99B-B2BC-4833-A0FC-6405C0C37F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35325" yWindow="330" windowWidth="18075" windowHeight="16995" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
+    <workbookView xWindow="30225" yWindow="585" windowWidth="18075" windowHeight="16995" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>snow</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>ice melting t°</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>outlet</t>
   </si>
 </sst>
 </file>
@@ -431,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6831DD79-7A46-42D6-B99E-96EB9F95B726}">
-  <dimension ref="B1:M16"/>
+  <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
@@ -453,7 +459,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -467,7 +473,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
@@ -475,7 +481,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -483,7 +489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -505,8 +511,14 @@
       <c r="J6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0</v>
       </c>
@@ -534,8 +546,11 @@
         <f>F7+H7+J7*$M$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>58849</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>10</v>
       </c>
@@ -564,8 +579,11 @@
         <f t="shared" ref="L8:L16" si="1">F8+H8+J8*$M$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>58850</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>10</v>
       </c>
@@ -594,8 +612,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>58851</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>10</v>
       </c>
@@ -625,8 +646,11 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>58852</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -657,8 +681,11 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>58853</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>10</v>
       </c>
@@ -684,11 +711,14 @@
         <v>0</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="1"/>
+        <f>F12+H12+J12*$M$2</f>
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>58854</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -717,8 +747,11 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>58855</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>10</v>
       </c>
@@ -747,8 +780,11 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>58856</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>10</v>
       </c>
@@ -776,8 +812,11 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>58857</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>0</v>
       </c>
@@ -804,6 +843,9 @@
       <c r="L16" s="2">
         <f t="shared" si="1"/>
         <v>16</v>
+      </c>
+      <c r="N16">
+        <v>58858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding tests on water balance.
</commit_message>
<xml_diff>
--- a/core/tests/resources/glacier snowpack.xlsx
+++ b/core/tests/resources/glacier snowpack.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\hydrobricks\core\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8457A99B-B2BC-4833-A0FC-6405C0C37F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C062171-A294-479A-9416-540C1FBAEE4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30225" yWindow="585" windowWidth="18075" windowHeight="16995" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
+    <workbookView xWindow="29370" yWindow="870" windowWidth="18510" windowHeight="14145" activeTab="1" xr2:uid="{FF9CD0C7-29C1-4408-9888-CE2FC7AF6140}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="model 1" sheetId="2" r:id="rId1"/>
+    <sheet name="model 2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>snow</t>
   </si>
@@ -75,10 +76,13 @@
     <t>ice melting t°</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>outlet</t>
+  </si>
+  <si>
+    <t>time (mjd)</t>
+  </si>
+  <si>
+    <t>ProcessMeltTest::GlacierModelWithSnowpack</t>
   </si>
 </sst>
 </file>
@@ -88,8 +92,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,12 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,184 +449,544 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6831DD79-7A46-42D6-B99E-96EB9F95B726}">
-  <dimension ref="B1:N16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82BACD3-BDC5-49B8-803C-F584D5C1390F}">
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="L2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2">
-        <v>0.5</v>
-      </c>
-    </row>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>-2</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <f>IF(C9&gt;$C$4,(C9-$C$4)*$C$3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <f>E9</f>
+        <v>8</v>
+      </c>
+      <c r="J9" s="2">
+        <f>IF(I9&gt;0,0,IF(C9&gt;$C$6,(C9-$C$6)*$C$5,0))</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <f>F9+H9+J9*$M$4</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>58849</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10:F18" si="0">B10*(1-C10/2)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <f>MIN(IF(C10&gt;$C$4,(C10-$C$4)*$C$3,0), I9)</f>
+        <v>4</v>
+      </c>
+      <c r="I10" s="2">
+        <f>I9+E10-H10</f>
+        <v>4</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" ref="J10:J18" si="1">IF(I10&gt;0,0,IF(C10&gt;$C$6,(C10-$C$6)*$C$5,0))</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <f t="shared" ref="L10:L18" si="2">F10+H10+J10*$M$4</f>
+        <v>4</v>
+      </c>
+      <c r="N10">
+        <v>58850</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" ref="H11:H18" si="3">MIN(IF(C11&gt;$C$4,(C11-$C$4)*$C$3,0), I10)</f>
+        <v>4</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" ref="I11:I16" si="4">I10+E11-H11</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>58851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L12" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <v>58852</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f>B13*(1-C13/2)</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N13">
+        <v>58853</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L14" s="2">
+        <f>F14+H14+J14*$M$4</f>
+        <v>6</v>
+      </c>
+      <c r="N14" s="3">
+        <v>58854</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>58855</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N16">
+        <v>58856</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L17" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N17">
+        <v>58857</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N18">
+        <v>58858</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6831DD79-7A46-42D6-B99E-96EB9F95B726}">
+  <dimension ref="B3:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="L4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="I6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
         <v>8</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" t="s">
         <v>14</v>
-      </c>
-      <c r="N6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>-2</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <f>IF(C7&gt;$C$2,(C7-$C$2)*$C$1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0</v>
-      </c>
-      <c r="J7" s="2">
-        <f>IF(I7&gt;0,0,IF(C7&gt;$C$4,(C7-$C$4)*$C$3,0))</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <f>F7+H7+J7*$M$2</f>
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>58849</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>-1</v>
-      </c>
-      <c r="E8">
-        <v>10</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <f>MIN(IF(C8&gt;$C$2,(C8-$C$2)*$C$1,0), I7)</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <f>I7+E8-H8</f>
-        <v>10</v>
-      </c>
-      <c r="J8" s="2">
-        <f t="shared" ref="J8:J16" si="0">IF(I8&gt;0,0,IF(C8&gt;$C$4,(C8-$C$4)*$C$3,0))</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <f t="shared" ref="L8:L16" si="1">F8+H8+J8*$M$2</f>
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>58850</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" ref="H9:H16" si="2">MIN(IF(C9&gt;$C$2,(C9-$C$2)*$C$1,0), I8)</f>
+        <f>IF(C9&gt;$C$4,(C9-$C$4)*$C$3,0)</f>
         <v>0</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" ref="I9:I14" si="3">I8+E9-H9</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="0"/>
+        <f>IF(I9&gt;0,0,IF(C9&gt;$C$6,(C9-$C$6)*$C$5,0))</f>
         <v>0</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="1"/>
+        <f>F9+H9+J9*$M$4</f>
         <v>0</v>
       </c>
       <c r="N9">
-        <v>58851</v>
+        <v>58849</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -621,33 +994,32 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10" si="4">B10*(1-C10/2)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="2"/>
+        <f>MIN(IF(C10&gt;$C$4,(C10-$C$4)*$C$3,0), I9)</f>
         <v>0</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f>I9+E10-H10</f>
+        <v>10</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J10:J18" si="0">IF(I10&gt;0,0,IF(C10&gt;$C$6,(C10-$C$6)*$C$5,0))</f>
         <v>0</v>
       </c>
       <c r="L10" s="2">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f>F10+H10+J10*$M$4</f>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>58852</v>
+        <v>58850</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
@@ -655,34 +1027,32 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="E11">
-        <f>B11*(1-C11/2)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <f>B11*C11/2</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H11:H18" si="1">MIN(IF(C11&gt;$C$4,(C11-$C$4)*$C$3,0), I10)</f>
         <v>0</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="3"/>
-        <v>25</v>
+        <f t="shared" ref="I11:I16" si="2">I10+E11-H11</f>
+        <v>20</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L11" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f>F11+H11+J11*$M$4</f>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>58853</v>
+        <v>58851</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -690,32 +1060,33 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <f t="shared" ref="E12" si="3">B12*(1-C12/2)</f>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
         <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="3"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L12" s="2">
-        <f>F12+H12+J12*$M$2</f>
-        <v>13</v>
+        <f>F12+H12+J12*$M$4</f>
+        <v>5</v>
       </c>
       <c r="N12">
-        <v>58854</v>
+        <v>58852</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -723,32 +1094,34 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E13">
+        <f>B13*(1-C13/2)</f>
         <v>0</v>
       </c>
       <c r="F13">
+        <f>B13*C13/2</f>
         <v>10</v>
       </c>
       <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="3"/>
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <f>F13+H13+J13*$M$4</f>
+        <v>10</v>
       </c>
       <c r="N13">
-        <v>58855</v>
+        <v>58853</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -756,7 +1129,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -765,23 +1138,23 @@
         <v>10</v>
       </c>
       <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="I14" s="2">
-        <f t="shared" si="3"/>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="N14">
-        <v>58856</v>
+        <f>F14+H14+J14*$M$4</f>
+        <v>13</v>
+      </c>
+      <c r="N14" s="3">
+        <v>58854</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -789,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -798,57 +1171,124 @@
         <v>10</v>
       </c>
       <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <f>F15+H15+J15*$M$4</f>
+        <v>16</v>
+      </c>
+      <c r="N15">
+        <v>58855</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I16" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="I15" s="2">
-        <v>0</v>
-      </c>
-      <c r="J15" s="2">
+      <c r="J16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <f>F16+H16+J16*$M$4</f>
+        <v>19</v>
+      </c>
+      <c r="N16">
+        <v>58856</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="L15" s="2">
-        <f t="shared" si="1"/>
+      <c r="L17" s="2">
+        <f>F17+H17+J17*$M$4</f>
         <v>31</v>
       </c>
-      <c r="N15">
+      <c r="N17">
         <v>58857</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
         <v>9</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0</v>
-      </c>
-      <c r="J16" s="2">
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="L16" s="2">
-        <f t="shared" si="1"/>
+      <c r="L18" s="2">
+        <f>F18+H18+J18*$M$4</f>
         <v>16</v>
       </c>
-      <c r="N16">
+      <c r="N18">
         <v>58858</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>